<commit_message>
added data to file
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -8,7 +8,8 @@
   </bookViews>
   <sheets>
     <sheet name="Accidents" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="roundabout road 1 lane" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="junction road 1 lane" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="straight road 2 lanes" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -467,7 +468,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -493,30 +494,35 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>Vehicle count in Plus Junction in last time stamp</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>Avg. Speed (Road 2, Direction 1)</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Avg. Speed (Road 0, Direction 1)</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Avg. Speed (Road 1, Direction 0)</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Avg. Speed (Road 1, Direction 1)</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Avg. Speed (Road 2, Direction 0)</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Avg. Speed (Road 0, Direction 0)</t>
         </is>
@@ -525,125 +531,153 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2024-09-05 20:35:21</t>
+          <t>2024-09-05 22:00:26</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>42.16358785889262</v>
+        <v>41.5556004701413</v>
       </c>
       <c r="C2" t="n">
         <v>10</v>
       </c>
       <c r="D2" t="n">
-        <v>48.52174592943641</v>
+        <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>49.85403120213379</v>
+        <v>45.46784310177639</v>
       </c>
       <c r="F2" t="n">
-        <v>46.36967638222285</v>
+        <v>49.77413081422966</v>
       </c>
       <c r="G2" t="n">
-        <v>34.10150867946534</v>
+        <v>41.12680021475725</v>
       </c>
       <c r="H2" t="n">
-        <v>42.73876421230204</v>
+        <v>41.93699337804463</v>
       </c>
       <c r="I2" t="n">
-        <v>26.98617170724176</v>
+        <v>50.40583294549832</v>
+      </c>
+      <c r="J2" t="n">
+        <v>3.600646894576797</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2024-09-05 20:35:26</t>
+          <t>2024-09-05 22:00:31</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>43.6833825144029</v>
+        <v>37.55672800173495</v>
       </c>
       <c r="C3" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D3" t="n">
-        <v>45.40892946856432</v>
+        <v>1</v>
       </c>
       <c r="E3" t="n">
-        <v>47.4148952695177</v>
+        <v>45.46784310177639</v>
       </c>
       <c r="F3" t="n">
-        <v>45.94831314861812</v>
+        <v>44.99773386020145</v>
       </c>
       <c r="G3" t="n">
-        <v>37.93516227686484</v>
+        <v>34.86979835085188</v>
       </c>
       <c r="H3" t="n">
-        <v>42.26840364095384</v>
+        <v>42.4491405187034</v>
       </c>
       <c r="I3" t="n">
-        <v>39.69047493522426</v>
+        <v>37.58831652549469</v>
+      </c>
+      <c r="J3" t="n">
+        <v>15.34775738813367</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>2024-09-05 20:35:31</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>36.72849993824526</v>
-      </c>
-      <c r="C4" t="n">
-        <v>23</v>
-      </c>
-      <c r="D4" t="n">
-        <v>42.31067591697889</v>
-      </c>
-      <c r="E4" t="n">
-        <v>32.34149427364297</v>
-      </c>
-      <c r="F4" t="n">
-        <v>36.49179715062975</v>
-      </c>
-      <c r="G4" t="n">
-        <v>38.7057001341238</v>
-      </c>
-      <c r="H4" t="n">
-        <v>41.1028080727787</v>
-      </c>
-      <c r="I4" t="n">
-        <v>30.38209236006155</v>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Time Stamp</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Average Speed</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Density</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Avg. Speed (Road 0, Direction 0)</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Avg. Speed (Road 0, Direction 1)</t>
+        </is>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>2024-09-05 20:35:36</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>32.1582331470202</v>
-      </c>
-      <c r="C5" t="n">
-        <v>26</v>
-      </c>
-      <c r="D5" t="n">
-        <v>39.31923081597413</v>
-      </c>
-      <c r="E5" t="n">
-        <v>38.7744894845075</v>
-      </c>
-      <c r="F5" t="n">
-        <v>40.06216843112183</v>
-      </c>
-      <c r="G5" t="n">
-        <v>30.59928583570115</v>
-      </c>
-      <c r="H5" t="n">
-        <v>23.35177679580869</v>
-      </c>
-      <c r="I5" t="n">
-        <v>21.09923198562685</v>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2024-09-05 22:00:41</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>72.17388803611196</v>
+      </c>
+      <c r="C2" t="n">
+        <v>12</v>
+      </c>
+      <c r="D2" t="n">
+        <v>75.82425041078419</v>
+      </c>
+      <c r="E2" t="n">
+        <v>68.52352566143973</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2024-09-05 22:00:46</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>73.14244518124306</v>
+      </c>
+      <c r="C3" t="n">
+        <v>19</v>
+      </c>
+      <c r="D3" t="n">
+        <v>76.00193087164676</v>
+      </c>
+      <c r="E3" t="n">
+        <v>69.96523885857228</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
work on traffic lights and roundabout
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -9,7 +9,6 @@
   <sheets>
     <sheet name="Accidents" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="junction road 1 lane" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="straight road 2 lanes" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -468,7 +467,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -531,11 +530,11 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2024-09-05 22:00:26</t>
+          <t>2024-09-08 16:17:33</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>41.5556004701413</v>
+        <v>43.02647959044286</v>
       </c>
       <c r="C2" t="n">
         <v>10</v>
@@ -544,140 +543,1344 @@
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>45.46784310177639</v>
+        <v>48.31806025790905</v>
       </c>
       <c r="F2" t="n">
-        <v>49.77413081422966</v>
+        <v>42.58823723084671</v>
       </c>
       <c r="G2" t="n">
-        <v>41.12680021475725</v>
+        <v>48.85609399093367</v>
       </c>
       <c r="H2" t="n">
-        <v>41.93699337804463</v>
+        <v>46.63900483709776</v>
       </c>
       <c r="I2" t="n">
-        <v>50.40583294549832</v>
+        <v>40.22477744900785</v>
       </c>
       <c r="J2" t="n">
-        <v>3.600646894576797</v>
+        <v>25.33050863074765</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2024-09-05 22:00:31</t>
+          <t>2024-09-08 16:17:38</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>37.55672800173495</v>
+        <v>38.8807140918198</v>
       </c>
       <c r="C3" t="n">
         <v>17</v>
       </c>
       <c r="D3" t="n">
+        <v>2</v>
+      </c>
+      <c r="E3" t="n">
+        <v>48.31806025790905</v>
+      </c>
+      <c r="F3" t="n">
+        <v>42.19294012244513</v>
+      </c>
+      <c r="G3" t="n">
+        <v>49.7292656079286</v>
+      </c>
+      <c r="H3" t="n">
+        <v>28.09700354651773</v>
+      </c>
+      <c r="I3" t="n">
+        <v>38.89279313936009</v>
+      </c>
+      <c r="J3" t="n">
+        <v>23.64800665349215</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2024-09-08 16:17:43</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>29.98722366673477</v>
+      </c>
+      <c r="C4" t="n">
+        <v>24</v>
+      </c>
+      <c r="D4" t="n">
+        <v>2</v>
+      </c>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="n">
+        <v>34.11925214264893</v>
+      </c>
+      <c r="G4" t="n">
+        <v>29.28351124040681</v>
+      </c>
+      <c r="H4" t="n">
+        <v>24.79134553217337</v>
+      </c>
+      <c r="I4" t="n">
+        <v>38.32484335369664</v>
+      </c>
+      <c r="J4" t="n">
+        <v>20.76908704161077</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2024-09-08 16:17:48</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>27.14204931251981</v>
+      </c>
+      <c r="C5" t="n">
+        <v>30</v>
+      </c>
+      <c r="D5" t="n">
+        <v>2</v>
+      </c>
+      <c r="E5" t="n">
+        <v>56.37646477545264</v>
+      </c>
+      <c r="F5" t="n">
+        <v>22.80722840402465</v>
+      </c>
+      <c r="G5" t="n">
+        <v>30.50756331532606</v>
+      </c>
+      <c r="H5" t="n">
+        <v>20.96509361927064</v>
+      </c>
+      <c r="I5" t="n">
+        <v>35.90897739248024</v>
+      </c>
+      <c r="J5" t="n">
+        <v>16.00721128548316</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2024-09-08 16:17:53</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>21.14724824393841</v>
+      </c>
+      <c r="C6" t="n">
+        <v>30</v>
+      </c>
+      <c r="D6" t="n">
+        <v>2</v>
+      </c>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="n">
+        <v>9.653787580190148</v>
+      </c>
+      <c r="G6" t="n">
+        <v>42.9985263986644</v>
+      </c>
+      <c r="H6" t="n">
+        <v>7.653694157108525</v>
+      </c>
+      <c r="I6" t="n">
+        <v>39.62142512034485</v>
+      </c>
+      <c r="J6" t="n">
+        <v>24.49585218901231</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2024-09-08 16:17:58</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>19.75412198506353</v>
+      </c>
+      <c r="C7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D7" t="n">
+        <v>3</v>
+      </c>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="n">
+        <v>15.51540357211055</v>
+      </c>
+      <c r="G7" t="n">
+        <v>40.06040013707663</v>
+      </c>
+      <c r="H7" t="n">
+        <v>3.133928439447313</v>
+      </c>
+      <c r="I7" t="n">
+        <v>15.9617269435552</v>
+      </c>
+      <c r="J7" t="n">
+        <v>28.47072466044194</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2024-09-08 16:18:03</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>17.06913809581569</v>
+      </c>
+      <c r="C8" t="n">
+        <v>30</v>
+      </c>
+      <c r="D8" t="n">
         <v>1</v>
       </c>
-      <c r="E3" t="n">
-        <v>45.46784310177639</v>
-      </c>
-      <c r="F3" t="n">
-        <v>44.99773386020145</v>
-      </c>
-      <c r="G3" t="n">
-        <v>34.86979835085188</v>
-      </c>
-      <c r="H3" t="n">
-        <v>42.4491405187034</v>
-      </c>
-      <c r="I3" t="n">
-        <v>37.58831652549469</v>
-      </c>
-      <c r="J3" t="n">
-        <v>15.34775738813367</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Time Stamp</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Average Speed</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Density</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Avg. Speed (Road 0, Direction 0)</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Avg. Speed (Road 0, Direction 1)</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>2024-09-05 22:00:41</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>72.17388803611196</v>
-      </c>
-      <c r="C2" t="n">
-        <v>12</v>
-      </c>
-      <c r="D2" t="n">
-        <v>75.82425041078419</v>
-      </c>
-      <c r="E2" t="n">
-        <v>68.52352566143973</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2024-09-05 22:00:46</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>73.14244518124306</v>
-      </c>
-      <c r="C3" t="n">
-        <v>19</v>
-      </c>
-      <c r="D3" t="n">
-        <v>76.00193087164676</v>
-      </c>
-      <c r="E3" t="n">
-        <v>69.96523885857228</v>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="n">
+        <v>10.73642207394417</v>
+      </c>
+      <c r="G8" t="n">
+        <v>37.70680927876905</v>
+      </c>
+      <c r="H8" t="n">
+        <v>5.736047030094884</v>
+      </c>
+      <c r="I8" t="n">
+        <v>45.30253485860182</v>
+      </c>
+      <c r="J8" t="n">
+        <v>17.45563107261079</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2024-09-08 16:18:08</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>16.06968762280583</v>
+      </c>
+      <c r="C9" t="n">
+        <v>30</v>
+      </c>
+      <c r="D9" t="n">
+        <v>2</v>
+      </c>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="n">
+        <v>12.88547766638684</v>
+      </c>
+      <c r="G9" t="n">
+        <v>29.19678652698718</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" t="n">
+        <v>32.69192948524864</v>
+      </c>
+      <c r="J9" t="n">
+        <v>28.51080782364341</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2024-09-08 16:18:13</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>13.48128867032793</v>
+      </c>
+      <c r="C10" t="n">
+        <v>30</v>
+      </c>
+      <c r="D10" t="n">
+        <v>3</v>
+      </c>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="n">
+        <v>3.60650300600014</v>
+      </c>
+      <c r="G10" t="n">
+        <v>23.23683022305168</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" t="n">
+        <v>50.86421234950349</v>
+      </c>
+      <c r="J10" t="n">
+        <v>33.55421109751246</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2024-09-08 16:18:18</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>15.25780578096973</v>
+      </c>
+      <c r="C11" t="n">
+        <v>30</v>
+      </c>
+      <c r="D11" t="n">
+        <v>2</v>
+      </c>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="n">
+        <v>3.60650300600014</v>
+      </c>
+      <c r="G11" t="n">
+        <v>28.59526908959215</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0</v>
+      </c>
+      <c r="I11" t="inlineStr"/>
+      <c r="J11" t="n">
+        <v>39.81325684587569</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2024-09-08 16:18:23</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>14.60400783167934</v>
+      </c>
+      <c r="C12" t="n">
+        <v>30</v>
+      </c>
+      <c r="D12" t="n">
+        <v>2</v>
+      </c>
+      <c r="E12" t="n">
+        <v>40.60539087524357</v>
+      </c>
+      <c r="F12" t="n">
+        <v>1.733761296245537</v>
+      </c>
+      <c r="G12" t="n">
+        <v>36.59780613933892</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0</v>
+      </c>
+      <c r="I12" t="inlineStr"/>
+      <c r="J12" t="n">
+        <v>33.39800093647508</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2024-09-08 16:18:28</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>17.75481681096813</v>
+      </c>
+      <c r="C13" t="n">
+        <v>30</v>
+      </c>
+      <c r="D13" t="n">
+        <v>1</v>
+      </c>
+      <c r="E13" t="n">
+        <v>40.28781629343516</v>
+      </c>
+      <c r="F13" t="n">
+        <v>11.08909774180106</v>
+      </c>
+      <c r="G13" t="n">
+        <v>41.35832055465209</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0</v>
+      </c>
+      <c r="I13" t="n">
+        <v>47.17639558934222</v>
+      </c>
+      <c r="J13" t="n">
+        <v>31.76748786581268</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2024-09-08 16:18:33</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>24.78584977721205</v>
+      </c>
+      <c r="C14" t="n">
+        <v>30</v>
+      </c>
+      <c r="D14" t="n">
+        <v>2</v>
+      </c>
+      <c r="E14" t="n">
+        <v>45.28907938804834</v>
+      </c>
+      <c r="F14" t="n">
+        <v>26.81455606715244</v>
+      </c>
+      <c r="G14" t="n">
+        <v>40.78580938539599</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0</v>
+      </c>
+      <c r="I14" t="n">
+        <v>42.24512338458115</v>
+      </c>
+      <c r="J14" t="n">
+        <v>25.98598561723408</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2024-09-08 16:18:38</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>21.06576961928717</v>
+      </c>
+      <c r="C15" t="n">
+        <v>30</v>
+      </c>
+      <c r="D15" t="n">
+        <v>2</v>
+      </c>
+      <c r="E15" t="n">
+        <v>51.35556050093366</v>
+      </c>
+      <c r="F15" t="n">
+        <v>19.26276004352849</v>
+      </c>
+      <c r="G15" t="n">
+        <v>35.88350236270925</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0</v>
+      </c>
+      <c r="I15" t="n">
+        <v>18.65692558991004</v>
+      </c>
+      <c r="J15" t="n">
+        <v>34.42742060963861</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2024-09-08 16:18:43</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>15.49930000424042</v>
+      </c>
+      <c r="C16" t="n">
+        <v>29</v>
+      </c>
+      <c r="D16" t="n">
+        <v>2</v>
+      </c>
+      <c r="E16" t="inlineStr"/>
+      <c r="F16" t="n">
+        <v>8.52418870532296</v>
+      </c>
+      <c r="G16" t="n">
+        <v>36.68165948339477</v>
+      </c>
+      <c r="H16" t="n">
+        <v>5.651579149944832</v>
+      </c>
+      <c r="I16" t="n">
+        <v>38.78269298765915</v>
+      </c>
+      <c r="J16" t="n">
+        <v>8.080815516625053</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2024-09-08 16:18:48</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>13.26267102338266</v>
+      </c>
+      <c r="C17" t="n">
+        <v>30</v>
+      </c>
+      <c r="D17" t="n">
+        <v>1</v>
+      </c>
+      <c r="E17" t="n">
+        <v>51.4505141629658</v>
+      </c>
+      <c r="F17" t="n">
+        <v>6.740236981823605</v>
+      </c>
+      <c r="G17" t="n">
+        <v>37.98410658236784</v>
+      </c>
+      <c r="H17" t="n">
+        <v>5.651579149944832</v>
+      </c>
+      <c r="I17" t="n">
+        <v>20.12576739774912</v>
+      </c>
+      <c r="J17" t="n">
+        <v>14.79183596563456</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2024-09-08 16:18:53</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>12.88334065515127</v>
+      </c>
+      <c r="C18" t="n">
+        <v>30</v>
+      </c>
+      <c r="D18" t="n">
+        <v>1</v>
+      </c>
+      <c r="E18" t="n">
+        <v>51.69460354128856</v>
+      </c>
+      <c r="F18" t="n">
+        <v>9.6998033479494</v>
+      </c>
+      <c r="G18" t="n">
+        <v>23.84284327395605</v>
+      </c>
+      <c r="H18" t="n">
+        <v>0</v>
+      </c>
+      <c r="I18" t="n">
+        <v>19.97842101424716</v>
+      </c>
+      <c r="J18" t="n">
+        <v>14.92552144842087</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2024-09-08 16:18:58</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>13.13080678209201</v>
+      </c>
+      <c r="C19" t="n">
+        <v>30</v>
+      </c>
+      <c r="D19" t="n">
+        <v>3</v>
+      </c>
+      <c r="E19" t="n">
+        <v>51.93869291961133</v>
+      </c>
+      <c r="F19" t="n">
+        <v>3.731385117982008</v>
+      </c>
+      <c r="G19" t="n">
+        <v>21.17322631406541</v>
+      </c>
+      <c r="H19" t="n">
+        <v>0</v>
+      </c>
+      <c r="I19" t="n">
+        <v>25.82135243817233</v>
+      </c>
+      <c r="J19" t="n">
+        <v>32.35956694481582</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>2024-09-08 16:19:03</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>14.49740592633243</v>
+      </c>
+      <c r="C20" t="n">
+        <v>30</v>
+      </c>
+      <c r="D20" t="n">
+        <v>1</v>
+      </c>
+      <c r="E20" t="n">
+        <v>46.50863962573752</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.7781716699879578</v>
+      </c>
+      <c r="G20" t="n">
+        <v>34.39981707896058</v>
+      </c>
+      <c r="H20" t="n">
+        <v>5.241821732149136</v>
+      </c>
+      <c r="I20" t="n">
+        <v>49.07607276224535</v>
+      </c>
+      <c r="J20" t="n">
+        <v>29.3560169593852</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>2024-09-08 16:19:08</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>16.5048226665135</v>
+      </c>
+      <c r="C21" t="n">
+        <v>30</v>
+      </c>
+      <c r="D21" t="n">
+        <v>3</v>
+      </c>
+      <c r="E21" t="n">
+        <v>48.90360453909587</v>
+      </c>
+      <c r="F21" t="n">
+        <v>6.043926808347766</v>
+      </c>
+      <c r="G21" t="n">
+        <v>42.36580475010679</v>
+      </c>
+      <c r="H21" t="n">
+        <v>0</v>
+      </c>
+      <c r="I21" t="n">
+        <v>49.07607276224535</v>
+      </c>
+      <c r="J21" t="n">
+        <v>38.89474528411466</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>2024-09-08 16:19:13</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>18.93533275874463</v>
+      </c>
+      <c r="C22" t="n">
+        <v>30</v>
+      </c>
+      <c r="D22" t="n">
+        <v>3</v>
+      </c>
+      <c r="E22" t="n">
+        <v>51.29856945245421</v>
+      </c>
+      <c r="F22" t="n">
+        <v>20.78352422481919</v>
+      </c>
+      <c r="G22" t="n">
+        <v>22.63012819367374</v>
+      </c>
+      <c r="H22" t="n">
+        <v>4.472392755055359</v>
+      </c>
+      <c r="I22" t="n">
+        <v>31.46147110641605</v>
+      </c>
+      <c r="J22" t="n">
+        <v>31.9389330322797</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>2024-09-08 16:19:18</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>14.15871031155314</v>
+      </c>
+      <c r="C23" t="n">
+        <v>30</v>
+      </c>
+      <c r="D23" t="n">
+        <v>1</v>
+      </c>
+      <c r="E23" t="n">
+        <v>39.09035816528795</v>
+      </c>
+      <c r="F23" t="n">
+        <v>5.979808477680143</v>
+      </c>
+      <c r="G23" t="n">
+        <v>30.75888206325255</v>
+      </c>
+      <c r="H23" t="n">
+        <v>4.472392755055359</v>
+      </c>
+      <c r="I23" t="inlineStr"/>
+      <c r="J23" t="n">
+        <v>28.9189182165919</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>2024-09-08 16:19:23</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>18.73542139226035</v>
+      </c>
+      <c r="C24" t="n">
+        <v>30</v>
+      </c>
+      <c r="D24" t="n">
+        <v>4</v>
+      </c>
+      <c r="E24" t="n">
+        <v>39.32539052566946</v>
+      </c>
+      <c r="F24" t="n">
+        <v>16.47657628619617</v>
+      </c>
+      <c r="G24" t="n">
+        <v>21.09882514613441</v>
+      </c>
+      <c r="H24" t="n">
+        <v>0</v>
+      </c>
+      <c r="I24" t="n">
+        <v>48.161750192558</v>
+      </c>
+      <c r="J24" t="n">
+        <v>45.48084486993956</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>2024-09-08 16:19:28</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>20.59194764380853</v>
+      </c>
+      <c r="C25" t="n">
+        <v>30</v>
+      </c>
+      <c r="D25" t="n">
+        <v>1</v>
+      </c>
+      <c r="E25" t="n">
+        <v>41.07169849693044</v>
+      </c>
+      <c r="F25" t="n">
+        <v>16.43583095010759</v>
+      </c>
+      <c r="G25" t="n">
+        <v>39.15907635735064</v>
+      </c>
+      <c r="H25" t="n">
+        <v>0</v>
+      </c>
+      <c r="I25" t="n">
+        <v>48.161750192558</v>
+      </c>
+      <c r="J25" t="n">
+        <v>43.89146105252122</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>2024-09-08 16:19:33</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>14.74974015018318</v>
+      </c>
+      <c r="C26" t="n">
+        <v>30</v>
+      </c>
+      <c r="D26" t="n">
+        <v>1</v>
+      </c>
+      <c r="E26" t="n">
+        <v>43.37661206714262</v>
+      </c>
+      <c r="F26" t="n">
+        <v>3.299933605240143</v>
+      </c>
+      <c r="G26" t="n">
+        <v>26.97051962417041</v>
+      </c>
+      <c r="H26" t="n">
+        <v>0</v>
+      </c>
+      <c r="I26" t="inlineStr"/>
+      <c r="J26" t="n">
+        <v>39.03030795478295</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>2024-09-08 16:19:38</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>12.93706550714043</v>
+      </c>
+      <c r="C27" t="n">
+        <v>30</v>
+      </c>
+      <c r="D27" t="n">
+        <v>2</v>
+      </c>
+      <c r="E27" t="n">
+        <v>45.70761056490835</v>
+      </c>
+      <c r="F27" t="n">
+        <v>0</v>
+      </c>
+      <c r="G27" t="n">
+        <v>25.06626730394047</v>
+      </c>
+      <c r="H27" t="n">
+        <v>8.822701381035921</v>
+      </c>
+      <c r="I27" t="n">
+        <v>46.94469819563265</v>
+      </c>
+      <c r="J27" t="n">
+        <v>30.01143761595909</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>2024-09-08 16:19:43</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>11.98468259928867</v>
+      </c>
+      <c r="C28" t="n">
+        <v>30</v>
+      </c>
+      <c r="D28" t="n">
+        <v>1</v>
+      </c>
+      <c r="E28" t="inlineStr"/>
+      <c r="F28" t="n">
+        <v>0</v>
+      </c>
+      <c r="G28" t="n">
+        <v>25.19944790293872</v>
+      </c>
+      <c r="H28" t="n">
+        <v>8.859766157472979</v>
+      </c>
+      <c r="I28" t="n">
+        <v>40.38828167857395</v>
+      </c>
+      <c r="J28" t="n">
+        <v>24.49008987822688</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>2024-09-08 16:19:49</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>9.739233719320403</v>
+      </c>
+      <c r="C29" t="n">
+        <v>30</v>
+      </c>
+      <c r="D29" t="n">
+        <v>0</v>
+      </c>
+      <c r="E29" t="n">
+        <v>33.81927056727304</v>
+      </c>
+      <c r="F29" t="n">
+        <v>0</v>
+      </c>
+      <c r="G29" t="n">
+        <v>31.98953540370915</v>
+      </c>
+      <c r="H29" t="n">
+        <v>0</v>
+      </c>
+      <c r="I29" t="n">
+        <v>13.61183842620655</v>
+      </c>
+      <c r="J29" t="n">
+        <v>25.5850133114645</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>2024-09-08 16:19:54</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>13.43251627011791</v>
+      </c>
+      <c r="C30" t="n">
+        <v>30</v>
+      </c>
+      <c r="D30" t="n">
+        <v>3</v>
+      </c>
+      <c r="E30" t="n">
+        <v>43.44024307155979</v>
+      </c>
+      <c r="F30" t="n">
+        <v>0</v>
+      </c>
+      <c r="G30" t="n">
+        <v>37.60283746838569</v>
+      </c>
+      <c r="H30" t="n">
+        <v>0</v>
+      </c>
+      <c r="I30" t="n">
+        <v>33.88840068127523</v>
+      </c>
+      <c r="J30" t="n">
+        <v>32.63561690810819</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>2024-09-08 16:19:59</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>12.90163687404346</v>
+      </c>
+      <c r="C31" t="n">
+        <v>30</v>
+      </c>
+      <c r="D31" t="n">
+        <v>1</v>
+      </c>
+      <c r="E31" t="n">
+        <v>43.25971760735841</v>
+      </c>
+      <c r="F31" t="n">
+        <v>0</v>
+      </c>
+      <c r="G31" t="n">
+        <v>33.98330410604498</v>
+      </c>
+      <c r="H31" t="n">
+        <v>4.025222568264356</v>
+      </c>
+      <c r="I31" t="n">
+        <v>31.56339700200463</v>
+      </c>
+      <c r="J31" t="n">
+        <v>25.81279603458199</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>2024-09-08 16:20:04</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>15.1117167290183</v>
+      </c>
+      <c r="C32" t="n">
+        <v>30</v>
+      </c>
+      <c r="D32" t="n">
+        <v>3</v>
+      </c>
+      <c r="E32" t="n">
+        <v>37.91526865407495</v>
+      </c>
+      <c r="F32" t="n">
+        <v>3.305169497826088</v>
+      </c>
+      <c r="G32" t="n">
+        <v>45.81093140819734</v>
+      </c>
+      <c r="H32" t="n">
+        <v>0</v>
+      </c>
+      <c r="I32" t="n">
+        <v>42.85836732621932</v>
+      </c>
+      <c r="J32" t="n">
+        <v>37.32987521692603</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>2024-09-08 16:20:09</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>23.50710794581378</v>
+      </c>
+      <c r="C33" t="n">
+        <v>30</v>
+      </c>
+      <c r="D33" t="n">
+        <v>2</v>
+      </c>
+      <c r="E33" t="n">
+        <v>43.9354593573907</v>
+      </c>
+      <c r="F33" t="n">
+        <v>16.39073352270055</v>
+      </c>
+      <c r="G33" t="n">
+        <v>26.8812151450512</v>
+      </c>
+      <c r="H33" t="n">
+        <v>13.22981797416074</v>
+      </c>
+      <c r="I33" t="n">
+        <v>44.58315908153111</v>
+      </c>
+      <c r="J33" t="n">
+        <v>50.21092545709611</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>2024-09-08 16:20:14</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>21.09920376770292</v>
+      </c>
+      <c r="C34" t="n">
+        <v>30</v>
+      </c>
+      <c r="D34" t="n">
+        <v>3</v>
+      </c>
+      <c r="E34" t="n">
+        <v>37.43998007903427</v>
+      </c>
+      <c r="F34" t="n">
+        <v>20.77044723033594</v>
+      </c>
+      <c r="G34" t="n">
+        <v>38.9279036799863</v>
+      </c>
+      <c r="H34" t="n">
+        <v>9.575592905433775</v>
+      </c>
+      <c r="I34" t="n">
+        <v>15.94373163200832</v>
+      </c>
+      <c r="J34" t="n">
+        <v>27.14632734504048</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>2024-09-08 16:20:19</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>20.02285190232566</v>
+      </c>
+      <c r="C35" t="n">
+        <v>30</v>
+      </c>
+      <c r="D35" t="n">
+        <v>2</v>
+      </c>
+      <c r="E35" t="inlineStr"/>
+      <c r="F35" t="n">
+        <v>29.26690542422275</v>
+      </c>
+      <c r="G35" t="n">
+        <v>21.61671519023994</v>
+      </c>
+      <c r="H35" t="n">
+        <v>12.14107825562981</v>
+      </c>
+      <c r="I35" t="n">
+        <v>14.31991343299749</v>
+      </c>
+      <c r="J35" t="n">
+        <v>20.15318761370241</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>2024-09-08 16:20:24</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>15.60380826401066</v>
+      </c>
+      <c r="C36" t="n">
+        <v>30</v>
+      </c>
+      <c r="D36" t="n">
+        <v>1</v>
+      </c>
+      <c r="E36" t="inlineStr"/>
+      <c r="F36" t="n">
+        <v>11.98869301855441</v>
+      </c>
+      <c r="G36" t="n">
+        <v>35.90528035898877</v>
+      </c>
+      <c r="H36" t="n">
+        <v>10.03120932212809</v>
+      </c>
+      <c r="I36" t="n">
+        <v>21.07014814824727</v>
+      </c>
+      <c r="J36" t="n">
+        <v>10.43667923111831</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>2024-09-08 16:20:29</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>12.34844095122248</v>
+      </c>
+      <c r="C37" t="n">
+        <v>30</v>
+      </c>
+      <c r="D37" t="n">
+        <v>2</v>
+      </c>
+      <c r="E37" t="inlineStr"/>
+      <c r="F37" t="n">
+        <v>4.791201148398518</v>
+      </c>
+      <c r="G37" t="n">
+        <v>38.7039162702175</v>
+      </c>
+      <c r="H37" t="n">
+        <v>8.976606056282364</v>
+      </c>
+      <c r="I37" t="n">
+        <v>20.68344726973159</v>
+      </c>
+      <c r="J37" t="n">
+        <v>12.65038489671074</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>2024-09-08 16:20:34</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>18.37172311632013</v>
+      </c>
+      <c r="C38" t="n">
+        <v>30</v>
+      </c>
+      <c r="D38" t="n">
+        <v>2</v>
+      </c>
+      <c r="E38" t="inlineStr"/>
+      <c r="F38" t="n">
+        <v>28.8417382926113</v>
+      </c>
+      <c r="G38" t="n">
+        <v>43.67703077353726</v>
+      </c>
+      <c r="H38" t="n">
+        <v>0</v>
+      </c>
+      <c r="I38" t="n">
+        <v>15.2768256835719</v>
+      </c>
+      <c r="J38" t="n">
+        <v>11.83957478520625</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>2024-09-08 16:20:39</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>10.8611740917191</v>
+      </c>
+      <c r="C39" t="n">
+        <v>30</v>
+      </c>
+      <c r="D39" t="n">
+        <v>4</v>
+      </c>
+      <c r="E39" t="inlineStr"/>
+      <c r="F39" t="n">
+        <v>13.44447089353567</v>
+      </c>
+      <c r="G39" t="n">
+        <v>22.10476338251927</v>
+      </c>
+      <c r="H39" t="n">
+        <v>0</v>
+      </c>
+      <c r="I39" t="n">
+        <v>15.2768256835719</v>
+      </c>
+      <c r="J39" t="n">
+        <v>11.76424235482654</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>2024-09-08 16:20:44</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>13.36848853576953</v>
+      </c>
+      <c r="C40" t="n">
+        <v>30</v>
+      </c>
+      <c r="D40" t="n">
+        <v>2</v>
+      </c>
+      <c r="E40" t="inlineStr"/>
+      <c r="F40" t="n">
+        <v>7.983723354339313</v>
+      </c>
+      <c r="G40" t="n">
+        <v>12.50689855567204</v>
+      </c>
+      <c r="H40" t="n">
+        <v>9.020158664497297</v>
+      </c>
+      <c r="I40" t="n">
+        <v>0</v>
+      </c>
+      <c r="J40" t="n">
+        <v>34.91043115439707</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>2024-09-08 16:20:49</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>18.56899164915232</v>
+      </c>
+      <c r="C41" t="n">
+        <v>30</v>
+      </c>
+      <c r="D41" t="n">
+        <v>3</v>
+      </c>
+      <c r="E41" t="n">
+        <v>41.6813149326583</v>
+      </c>
+      <c r="F41" t="n">
+        <v>23.96900819786823</v>
+      </c>
+      <c r="G41" t="n">
+        <v>25.6707174129576</v>
+      </c>
+      <c r="H41" t="n">
+        <v>13.25699954214337</v>
+      </c>
+      <c r="I41" t="n">
+        <v>0</v>
+      </c>
+      <c r="J41" t="n">
+        <v>26.17664092457888</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>2024-09-08 16:20:54</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>18.44047756449406</v>
+      </c>
+      <c r="C42" t="n">
+        <v>30</v>
+      </c>
+      <c r="D42" t="n">
+        <v>2</v>
+      </c>
+      <c r="E42" t="n">
+        <v>40.71427867753857</v>
+      </c>
+      <c r="F42" t="n">
+        <v>17.14361123431702</v>
+      </c>
+      <c r="G42" t="n">
+        <v>51.34143482591521</v>
+      </c>
+      <c r="H42" t="n">
+        <v>5.766556959038756</v>
+      </c>
+      <c r="I42" t="n">
+        <v>0</v>
+      </c>
+      <c r="J42" t="n">
+        <v>46.41710662248497</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
place change of enter roundabout check
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -8,8 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Accidents" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="junction road 1 lane" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="roundabout road 1 lane" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="roundabout road 1 lane" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -468,7 +467,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -494,7 +493,7 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Vehicle count in plus-junction in last time stamp</t>
+          <t>Vehicle count in roundabout in last time stamp</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
@@ -531,404 +530,435 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2024-09-08 16:24:03</t>
+          <t>2024-09-08 21:21:41</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>47.9984422459021</v>
+        <v>42.65169408168538</v>
       </c>
       <c r="C2" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>67.21388277470335</v>
+        <v>27.50775354553763</v>
       </c>
       <c r="F2" t="n">
-        <v>47.79148407498812</v>
+        <v>48.93983740277298</v>
       </c>
       <c r="G2" t="n">
-        <v>43.59691816838983</v>
+        <v>45.98602974445519</v>
       </c>
       <c r="H2" t="n">
-        <v>44.05994984604792</v>
+        <v>41.09816980657508</v>
       </c>
       <c r="I2" t="n">
-        <v>52.73892425187688</v>
+        <v>35.72493134138826</v>
       </c>
       <c r="J2" t="n">
-        <v>32.79645253032055</v>
+        <v>47.0309636655257</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2024-09-08 16:24:08</t>
+          <t>2024-09-08 21:21:46</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>41.03814508507347</v>
+        <v>41.83239143394959</v>
       </c>
       <c r="C3" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D3" t="n">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="E3" t="n">
+        <v>41.18342263410457</v>
       </c>
       <c r="F3" t="n">
-        <v>48.62532813991869</v>
+        <v>45.66126563951377</v>
       </c>
       <c r="G3" t="n">
-        <v>38.29017738635937</v>
+        <v>37.37317891009498</v>
       </c>
       <c r="H3" t="n">
-        <v>48.10946569089126</v>
+        <v>42.63785745438945</v>
       </c>
       <c r="I3" t="n">
-        <v>23.42779827600332</v>
+        <v>43.35194283526967</v>
       </c>
       <c r="J3" t="n">
-        <v>40.52475672670661</v>
+        <v>30.56367101425228</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2024-09-08 16:24:13</t>
+          <t>2024-09-08 21:21:51</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>41.12565947882221</v>
+        <v>35.8775946347098</v>
       </c>
       <c r="C4" t="n">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D4" t="n">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="E4" t="n">
+        <v>42.23036052443546</v>
       </c>
       <c r="F4" t="n">
-        <v>46.73861514834219</v>
+        <v>36.57143032528116</v>
       </c>
       <c r="G4" t="n">
-        <v>47.3810717291498</v>
+        <v>37.09780653145859</v>
       </c>
       <c r="H4" t="n">
-        <v>42.3112025025311</v>
+        <v>38.75924134275367</v>
       </c>
       <c r="I4" t="n">
-        <v>48.60573432171556</v>
+        <v>29.40735349023602</v>
       </c>
       <c r="J4" t="n">
-        <v>20.57899426280818</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:J8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Time Stamp</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Average Speed</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Density</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Vehicle count in roundabout in last time stamp</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Avg. Speed (Road 1, Direction 0)</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Avg. Speed (Road 1, Direction 1)</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Avg. Speed (Road 2, Direction 0)</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Avg. Speed (Road 2, Direction 1)</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>Avg. Speed (Road 3, Direction 0)</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>Avg. Speed (Road 3, Direction 1)</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>2024-09-08 16:24:39</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>42.48968130282115</v>
-      </c>
-      <c r="C2" t="n">
-        <v>7</v>
-      </c>
-      <c r="D2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E2" t="n">
-        <v>37.77609569257863</v>
-      </c>
-      <c r="F2" t="n">
-        <v>43.85813789194631</v>
-      </c>
-      <c r="G2" t="n">
-        <v>38.70217513977165</v>
-      </c>
-      <c r="H2" t="n">
-        <v>51.60972263747655</v>
-      </c>
-      <c r="I2" t="n">
-        <v>43.84740417344995</v>
-      </c>
-      <c r="J2" t="inlineStr"/>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2024-09-08 16:24:44</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>38.09598667999036</v>
-      </c>
-      <c r="C3" t="n">
-        <v>13</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E3" t="n">
-        <v>25.01996034572543</v>
-      </c>
-      <c r="F3" t="n">
-        <v>46.1458409135554</v>
-      </c>
-      <c r="G3" t="n">
-        <v>40.43277175818153</v>
-      </c>
-      <c r="H3" t="n">
-        <v>24.29041326302687</v>
-      </c>
-      <c r="I3" t="n">
-        <v>44.61985030564972</v>
-      </c>
-      <c r="J3" t="n">
-        <v>41.93847184048598</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>2024-09-08 16:24:49</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>35.18627031198608</v>
-      </c>
-      <c r="C4" t="n">
-        <v>18</v>
-      </c>
-      <c r="D4" t="n">
-        <v>0</v>
-      </c>
-      <c r="E4" t="n">
-        <v>31.7224412971008</v>
-      </c>
-      <c r="F4" t="n">
-        <v>31.83235450670539</v>
-      </c>
-      <c r="G4" t="n">
-        <v>33.1478859371869</v>
-      </c>
-      <c r="H4" t="n">
-        <v>35.07741907509216</v>
-      </c>
-      <c r="I4" t="n">
-        <v>44.93252071394751</v>
-      </c>
-      <c r="J4" t="n">
-        <v>42.89917207833471</v>
+        <v>34.72340884384939</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2024-09-08 16:24:54</t>
+          <t>2024-09-08 21:21:56</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>29.57287697086588</v>
+        <v>34.19885530450585</v>
       </c>
       <c r="C5" t="n">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E5" t="n">
-        <v>22.91630280035401</v>
+        <v>43.16869640106486</v>
       </c>
       <c r="F5" t="n">
-        <v>23.77026837479247</v>
+        <v>32.54060551797654</v>
       </c>
       <c r="G5" t="n">
-        <v>20.95154887322694</v>
+        <v>31.87501599913109</v>
       </c>
       <c r="H5" t="n">
-        <v>34.40026617785907</v>
+        <v>24.01794782391335</v>
       </c>
       <c r="I5" t="n">
-        <v>45.17422153603508</v>
+        <v>38.36228172087432</v>
       </c>
       <c r="J5" t="n">
-        <v>44.56229683011883</v>
+        <v>35.38571454581499</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2024-09-08 16:24:59</t>
+          <t>2024-09-08 21:22:01</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>23.62890031908519</v>
+        <v>37.75012171357329</v>
       </c>
       <c r="C6" t="n">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D6" t="n">
         <v>1</v>
       </c>
       <c r="E6" t="n">
-        <v>7.740435027954331</v>
+        <v>38.15345396235678</v>
       </c>
       <c r="F6" t="n">
-        <v>22.12893373588828</v>
+        <v>38.75965777044865</v>
       </c>
       <c r="G6" t="n">
-        <v>27.45902786221881</v>
+        <v>43.00559318817272</v>
       </c>
       <c r="H6" t="n">
-        <v>30.79042074308569</v>
+        <v>28.10349144887012</v>
       </c>
       <c r="I6" t="n">
-        <v>38.06994752483914</v>
+        <v>40.85007664513808</v>
       </c>
       <c r="J6" t="n">
-        <v>44.77274025443793</v>
+        <v>39.90368313573591</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2024-09-08 16:25:04</t>
+          <t>2024-09-08 21:22:06</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>25.71543291403896</v>
+        <v>31.78718713402786</v>
       </c>
       <c r="C7" t="n">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D7" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E7" t="n">
-        <v>21.90715536892499</v>
+        <v>35.48945225984817</v>
       </c>
       <c r="F7" t="n">
-        <v>11.24819443593591</v>
+        <v>28.53493442662284</v>
       </c>
       <c r="G7" t="n">
-        <v>38.40980747124283</v>
+        <v>15.86757958348541</v>
       </c>
       <c r="H7" t="n">
-        <v>37.15413828556277</v>
+        <v>30.34660101975821</v>
       </c>
       <c r="I7" t="n">
-        <v>40.11248149384515</v>
+        <v>40.93314263359598</v>
       </c>
       <c r="J7" t="n">
-        <v>37.11784679648289</v>
+        <v>37.8845705775264</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2024-09-08 16:25:05</t>
+          <t>2024-09-08 21:22:11</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>23.023497877467</v>
+        <v>31.443238225486</v>
       </c>
       <c r="C8" t="n">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D8" t="n">
+        <v>3</v>
+      </c>
+      <c r="E8" t="n">
+        <v>47.63584882269483</v>
+      </c>
+      <c r="F8" t="n">
+        <v>35.01900615774418</v>
+      </c>
+      <c r="G8" t="n">
+        <v>24.7056553344296</v>
+      </c>
+      <c r="H8" t="n">
+        <v>34.30495800640912</v>
+      </c>
+      <c r="I8" t="n">
+        <v>38.90346985563132</v>
+      </c>
+      <c r="J8" t="n">
+        <v>21.31086759029264</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2024-09-08 21:22:16</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>21.87835704970522</v>
+      </c>
+      <c r="C9" t="n">
+        <v>29</v>
+      </c>
+      <c r="D9" t="n">
         <v>0</v>
       </c>
-      <c r="E8" t="n">
-        <v>13.38092558406077</v>
-      </c>
-      <c r="F8" t="n">
-        <v>12.02309048441934</v>
-      </c>
-      <c r="G8" t="n">
-        <v>28.47677361058864</v>
-      </c>
-      <c r="H8" t="n">
-        <v>37.15413828556277</v>
-      </c>
-      <c r="I8" t="n">
-        <v>44.46764588008612</v>
-      </c>
-      <c r="J8" t="n">
-        <v>35.41492701908262</v>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="n">
+        <v>15.44126228361442</v>
+      </c>
+      <c r="G9" t="n">
+        <v>20.40919447008739</v>
+      </c>
+      <c r="H9" t="n">
+        <v>29.66779133677761</v>
+      </c>
+      <c r="I9" t="n">
+        <v>37.75602962725852</v>
+      </c>
+      <c r="J9" t="n">
+        <v>16.20204207492839</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2024-09-08 21:22:21</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>25.17554947835098</v>
+      </c>
+      <c r="C10" t="n">
+        <v>30</v>
+      </c>
+      <c r="D10" t="n">
+        <v>4</v>
+      </c>
+      <c r="E10" t="n">
+        <v>53.99856926496221</v>
+      </c>
+      <c r="F10" t="n">
+        <v>21.3771642022856</v>
+      </c>
+      <c r="G10" t="n">
+        <v>38.36214637831103</v>
+      </c>
+      <c r="H10" t="n">
+        <v>22.14968431396526</v>
+      </c>
+      <c r="I10" t="n">
+        <v>31.37471965599239</v>
+      </c>
+      <c r="J10" t="n">
+        <v>13.46923419660759</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2024-09-08 21:22:26</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>21.09993557859023</v>
+      </c>
+      <c r="C11" t="n">
+        <v>34</v>
+      </c>
+      <c r="D11" t="n">
+        <v>2</v>
+      </c>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="n">
+        <v>13.61322211922838</v>
+      </c>
+      <c r="G11" t="n">
+        <v>36.51457457911806</v>
+      </c>
+      <c r="H11" t="n">
+        <v>22.37350604756102</v>
+      </c>
+      <c r="I11" t="n">
+        <v>22.94937657682778</v>
+      </c>
+      <c r="J11" t="n">
+        <v>16.08776447232915</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2024-09-08 21:22:31</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>17.31889610160293</v>
+      </c>
+      <c r="C12" t="n">
+        <v>36</v>
+      </c>
+      <c r="D12" t="n">
+        <v>2</v>
+      </c>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="n">
+        <v>9.877188687671687</v>
+      </c>
+      <c r="G12" t="n">
+        <v>18.01061388887265</v>
+      </c>
+      <c r="H12" t="n">
+        <v>27.74934021368255</v>
+      </c>
+      <c r="I12" t="n">
+        <v>13.60757162405413</v>
+      </c>
+      <c r="J12" t="n">
+        <v>23.90219283099964</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2024-09-08 21:22:36</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>22.00647989742064</v>
+      </c>
+      <c r="C13" t="n">
+        <v>39</v>
+      </c>
+      <c r="D13" t="n">
+        <v>3</v>
+      </c>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="n">
+        <v>21.75933265954236</v>
+      </c>
+      <c r="G13" t="n">
+        <v>9.31871679266354</v>
+      </c>
+      <c r="H13" t="n">
+        <v>21.69908722927452</v>
+      </c>
+      <c r="I13" t="n">
+        <v>20.53021853630523</v>
+      </c>
+      <c r="J13" t="n">
+        <v>29.23242754024612</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2024-09-08 21:22:39</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>17.76975650380773</v>
+      </c>
+      <c r="C14" t="n">
+        <v>39</v>
+      </c>
+      <c r="D14" t="n">
+        <v>1</v>
+      </c>
+      <c r="E14" t="n">
+        <v>33.05762659292159</v>
+      </c>
+      <c r="F14" t="n">
+        <v>11.52772228210777</v>
+      </c>
+      <c r="G14" t="n">
+        <v>20.11841982118494</v>
+      </c>
+      <c r="H14" t="n">
+        <v>28.11787159012668</v>
+      </c>
+      <c r="I14" t="n">
+        <v>12.9776915357985</v>
+      </c>
+      <c r="J14" t="n">
+        <v>18.33503453179764</v>
       </c>
     </row>
   </sheetData>

</xml_diff>